<commit_message>
Full excel of test investments
</commit_message>
<xml_diff>
--- a/assets/dataScraped.xlsx
+++ b/assets/dataScraped.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>up or down</t>
+          <t>fluctuation</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -486,18 +486,18 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>75.86</t>
+          <t>74.49</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.19</v>
+        <v>1.56</v>
       </c>
       <c r="F2" t="n">
-        <v>0.26</v>
+        <v>2.05</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -642,14 +642,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>123.99</t>
+          <t>124.10</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -678,23 +678,23 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>38.39</t>
+          <t>37.61</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.32</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>0.84</v>
+        <v>2.1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>29.41 – 38.73</t>
+          <t>29.44 – 38.73</t>
         </is>
       </c>
     </row>
@@ -714,14 +714,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>120.07</t>
+          <t>120.18</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.12</v>
+        <v>0.01</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -750,18 +750,18 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>88.01</t>
+          <t>86.00</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.31</v>
+        <v>2.13</v>
       </c>
       <c r="F9" t="n">
-        <v>0.35</v>
+        <v>2.42</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -786,18 +786,18 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>19.53</t>
+          <t>19.02</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.09</v>
+        <v>0.47</v>
       </c>
       <c r="F10" t="n">
-        <v>0.47</v>
+        <v>2.43</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -822,18 +822,18 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>63.50</t>
+          <t>62.34</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.09</v>
+        <v>1.32</v>
       </c>
       <c r="F11" t="n">
-        <v>0.14</v>
+        <v>2.07</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -858,23 +858,23 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>$7.45</t>
+          <t>$7.30</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.01</v>
+        <v>0.14</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1</v>
+        <v>1.88</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>7.44 – 7.45</t>
+          <t>7.30 – 7.35</t>
         </is>
       </c>
     </row>
@@ -894,27 +894,23 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>$8.68</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Check manually</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Check manually</t>
-        </is>
+          <t>$8.43</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2.99</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>8.67 – 8.70</t>
+          <t>8.42 – 8.48</t>
         </is>
       </c>
     </row>
@@ -934,14 +930,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10.78</t>
+          <t>10.76</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="F14" t="n">
-        <v>0.03</v>
+        <v>0.16</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -970,14 +966,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4.92</t>
+          <t>4.95</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="F15" t="n">
-        <v>0.16</v>
+        <v>0.51</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1006,18 +1002,18 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>54.44</t>
+          <t>54.47</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="F16" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1082,18 +1078,18 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13.73</t>
+          <t>13.28</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.06</v>
+        <v>0.44</v>
       </c>
       <c r="F18" t="n">
-        <v>0.42</v>
+        <v>3.22</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1118,14 +1114,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>98.13</t>
+          <t>98.27</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.32</v>
+        <v>0.19</v>
       </c>
       <c r="F19" t="n">
-        <v>0.33</v>
+        <v>0.19</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1134,7 +1130,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>98.13 – 98.13</t>
+          <t>98.07 – 98.37</t>
         </is>
       </c>
     </row>
@@ -1154,23 +1150,23 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>$7.50</t>
+          <t>$7.26</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.04</v>
+        <v>0.25</v>
       </c>
       <c r="F20" t="n">
-        <v>0.48</v>
+        <v>3.29</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>7.49 – 7.52</t>
+          <t>7.18 – 7.33</t>
         </is>
       </c>
     </row>
@@ -1190,18 +1186,18 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>298.59</t>
+          <t>285.39</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.96</v>
+        <v>13.03</v>
       </c>
       <c r="F21" t="n">
-        <v>0.32</v>
+        <v>4.37</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1226,18 +1222,18 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>536.34</t>
+          <t>523.52</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.4</v>
+        <v>13.7</v>
       </c>
       <c r="F22" t="n">
-        <v>0.08</v>
+        <v>2.55</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1262,18 +1258,18 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>25.83</t>
+          <t>25.21</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.06</v>
+        <v>0.66</v>
       </c>
       <c r="F23" t="n">
-        <v>0.23</v>
+        <v>2.55</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1298,23 +1294,23 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>77.93</t>
+          <t>76.25</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.41</v>
+        <v>1.59</v>
       </c>
       <c r="F24" t="n">
-        <v>0.53</v>
+        <v>2.04</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>77.63 – 77.93</t>
+          <t>75.74 – 76.53</t>
         </is>
       </c>
     </row>
@@ -1334,27 +1330,23 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>54.00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Check manually</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Check manually</t>
-        </is>
+          <t>53.93</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.09</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>53.88 – 55.30</t>
+          <t>53.85 – 55.30</t>
         </is>
       </c>
     </row>
@@ -1374,14 +1366,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>27.06</t>
+          <t>27.23</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
       <c r="F26" t="n">
-        <v>0.13</v>
+        <v>0.59</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1410,14 +1402,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>5.24</t>
+          <t>5.26</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1</v>
+        <v>0.47</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1446,18 +1438,18 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13.02</t>
+          <t>12.72</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.03</v>
+        <v>0.35</v>
       </c>
       <c r="F28" t="n">
-        <v>0.22</v>
+        <v>2.69</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1482,18 +1474,18 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>34.24</t>
+          <t>33.57</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F29" t="n">
-        <v>0.3</v>
+        <v>2.01</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1518,18 +1510,18 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>20.21</t>
+          <t>19.77</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0.04</v>
+        <v>0.45</v>
       </c>
       <c r="F30" t="n">
-        <v>0.2</v>
+        <v>2.23</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1554,18 +1546,18 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>11.72</t>
+          <t>11.37</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.01</v>
+        <v>0.37</v>
       </c>
       <c r="F31" t="n">
-        <v>0.11</v>
+        <v>3.13</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1590,14 +1582,14 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>54.12</t>
+          <t>53.96</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.01</v>
+        <v>0.13</v>
       </c>
       <c r="F32" t="n">
-        <v>0.01</v>
+        <v>0.24</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1606,7 +1598,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>53.96 – 55.18</t>
+          <t>53.87 – 55.18</t>
         </is>
       </c>
     </row>
@@ -1746,18 +1738,18 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>24.22</t>
+          <t>23.45</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.05</v>
+        <v>0.78</v>
       </c>
       <c r="F36" t="n">
-        <v>0.19</v>
+        <v>3.2</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1782,18 +1774,18 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>434.93</t>
+          <t>425.42</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1.19</v>
+        <v>9.48</v>
       </c>
       <c r="F37" t="n">
-        <v>0.27</v>
+        <v>2.18</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1858,14 +1850,14 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>131.51</t>
+          <t>132.25</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.21</v>
+        <v>0.67</v>
       </c>
       <c r="F39" t="n">
-        <v>0.16</v>
+        <v>0.51</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1974,14 +1966,14 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>20.00</t>
+          <t>19.23</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.01</v>
+        <v>0.82</v>
       </c>
       <c r="F42" t="n">
-        <v>0.03</v>
+        <v>4.08</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -2010,23 +2002,23 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>90.50</t>
+          <t>89.17</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.4</v>
+        <v>1.42</v>
       </c>
       <c r="F43" t="n">
-        <v>0.44</v>
+        <v>1.57</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>62.75 – 96.32</t>
+          <t>63.56 – 96.32</t>
         </is>
       </c>
     </row>
@@ -2046,18 +2038,18 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>155.72</t>
+          <t>155.32</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
       <c r="F44" t="n">
-        <v>0.08</v>
+        <v>0.13</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2082,18 +2074,18 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>15.33</t>
+          <t>15.02</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.12</v>
+        <v>0.34</v>
       </c>
       <c r="F45" t="n">
-        <v>0.79</v>
+        <v>2.19</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2118,14 +2110,14 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>$5.83</t>
+          <t>$5.80</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="F46" t="n">
-        <v>0.1</v>
+        <v>0.55</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2134,7 +2126,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>5.82 – 5.83</t>
+          <t>5.80 – 5.83</t>
         </is>
       </c>
     </row>
@@ -2154,14 +2146,14 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>54.12</t>
+          <t>53.96</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.01</v>
+        <v>0.13</v>
       </c>
       <c r="F47" t="n">
-        <v>0.01</v>
+        <v>0.24</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2170,7 +2162,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>53.96 – 55.18</t>
+          <t>53.87 – 55.18</t>
         </is>
       </c>
     </row>
@@ -2194,10 +2186,10 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.67</v>
+        <v>0.06</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2206,7 +2198,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>6.96 – 7.04</t>
+          <t>7.02 – 7.02</t>
         </is>
       </c>
     </row>
@@ -2226,18 +2218,18 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>38.39</t>
+          <t>37.36</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.14</v>
+        <v>1.06</v>
       </c>
       <c r="F49" t="n">
-        <v>0.37</v>
+        <v>2.76</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2262,14 +2254,14 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>123.99</t>
+          <t>124.06</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="F50" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2298,23 +2290,23 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>$34.29</t>
+          <t>$33.58</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.16</v>
+        <v>0.7</v>
       </c>
       <c r="F51" t="n">
-        <v>0.47</v>
+        <v>2.03</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>34.27 – 34.29</t>
+          <t>33.58 – 33.58</t>
         </is>
       </c>
     </row>
@@ -2374,23 +2366,23 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>$9.25</t>
+          <t>$9.07</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0.05</v>
+        <v>0.17</v>
       </c>
       <c r="F53" t="n">
-        <v>0.49</v>
+        <v>1.89</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>9.25 – 9.26</t>
+          <t>9.05 – 9.13</t>
         </is>
       </c>
     </row>
@@ -2490,18 +2482,18 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>171.50</t>
+          <t>171.15</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>0.71</v>
+        <v>0.61</v>
       </c>
       <c r="F56" t="n">
-        <v>0.42</v>
+        <v>0.36</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2526,18 +2518,18 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>10.82</t>
+          <t>10.95</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
       <c r="F57" t="n">
-        <v>0.09</v>
+        <v>1.01</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2562,18 +2554,18 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>60.82</t>
+          <t>60.36</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>0.34</v>
+        <v>1.15</v>
       </c>
       <c r="F58" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.87</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2598,18 +2590,18 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>265.55</t>
+          <t>260.00</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>0.87</v>
+        <v>5.85</v>
       </c>
       <c r="F59" t="n">
-        <v>0.33</v>
+        <v>2.2</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2634,18 +2626,18 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>125.80</t>
+          <t>123.32</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>0.38</v>
+        <v>2.6</v>
       </c>
       <c r="F60" t="n">
-        <v>0.3</v>
+        <v>2.06</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -2710,14 +2702,14 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>$133.06</t>
+          <t>$133.34</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0.04</v>
+        <v>0.28</v>
       </c>
       <c r="F62" t="n">
-        <v>0.03</v>
+        <v>0.21</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2746,14 +2738,14 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>5.00</t>
+          <t>4.99</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F63" t="n">
-        <v>0.05</v>
+        <v>0.13</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2782,18 +2774,18 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>134.92</t>
+          <t>135.23</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
       <c r="F64" t="n">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -2818,18 +2810,18 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>52.23</t>
+          <t>50.89</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.2</v>
+        <v>1.47</v>
       </c>
       <c r="F65" t="n">
-        <v>0.38</v>
+        <v>2.8</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -2854,18 +2846,18 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>118.32</t>
+          <t>115.95</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>0.61</v>
+        <v>2.29</v>
       </c>
       <c r="F66" t="n">
-        <v>0.52</v>
+        <v>1.94</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -2970,18 +2962,18 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>5.16</t>
+          <t>5.01</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="F69" t="n">
-        <v>0.07000000000000001</v>
+        <v>3.19</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -3166,23 +3158,23 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>407.90</t>
+          <t>402.15</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>2.4</v>
+        <v>5.85</v>
       </c>
       <c r="F74" t="n">
-        <v>0.59</v>
+        <v>1.43</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>302.60 – 414.70</t>
+          <t>302.70 – 414.70</t>
         </is>
       </c>
     </row>
@@ -3202,18 +3194,18 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>267.76</t>
+          <t>260.33</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.04</v>
+        <v>7.7</v>
       </c>
       <c r="F75" t="n">
-        <v>0.01</v>
+        <v>2.87</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -3238,18 +3230,18 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>414.85</t>
+          <t>409.75</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>1.25</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
-        <v>0.3</v>
+        <v>1.21</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -3314,18 +3306,18 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>12.79</t>
+          <t>12.33</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.03</v>
+        <v>0.42</v>
       </c>
       <c r="F78" t="n">
-        <v>0.23</v>
+        <v>3.33</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -3550,18 +3542,18 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>115.35</t>
+          <t>116.57</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.07000000000000001</v>
+        <v>1.27</v>
       </c>
       <c r="F84" t="n">
-        <v>0.06</v>
+        <v>1.1</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3586,14 +3578,14 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>323.52</t>
+          <t>323.17</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.91</v>
+        <v>1.3</v>
       </c>
       <c r="F85" t="n">
-        <v>0.28</v>
+        <v>0.4</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3622,18 +3614,18 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>73.19</t>
+          <t>71.16</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.4</v>
+        <v>1.92</v>
       </c>
       <c r="F86" t="n">
-        <v>0.55</v>
+        <v>2.63</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -3658,14 +3650,14 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>$43.22</t>
+          <t>$42.53</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.11</v>
+        <v>0.71</v>
       </c>
       <c r="F87" t="n">
-        <v>0.24</v>
+        <v>1.64</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3674,7 +3666,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>43.22 – 43.53</t>
+          <t>42.53 – 42.53</t>
         </is>
       </c>
     </row>
@@ -3694,23 +3686,23 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>$51.88</t>
+          <t>$51.01</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.01</v>
+        <v>0.86</v>
       </c>
       <c r="F88" t="n">
-        <v>0.02</v>
+        <v>1.66</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>51.82 – 51.91</t>
+          <t>50.88 – 51.10</t>
         </is>
       </c>
     </row>
@@ -3730,14 +3722,14 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>133.67</t>
+          <t>133.48</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.12</v>
+        <v>0.26</v>
       </c>
       <c r="F89" t="n">
-        <v>0.09</v>
+        <v>0.19</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -3746,7 +3738,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>133.65 – 133.86</t>
+          <t>133.40 – 133.91</t>
         </is>
       </c>
     </row>
@@ -3766,23 +3758,23 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>$88.56</t>
+          <t>$86.81</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>0.41</v>
+        <v>1.72</v>
       </c>
       <c r="F90" t="n">
-        <v>0.47</v>
+        <v>1.94</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>88.44 – 88.71</t>
+          <t>86.40 – 87.59</t>
         </is>
       </c>
     </row>
@@ -3802,14 +3794,14 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>272.80</t>
+          <t>275.86</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0.86</v>
+        <v>2.93</v>
       </c>
       <c r="F91" t="n">
-        <v>0.32</v>
+        <v>1.07</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3838,14 +3830,14 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>$125.67</t>
+          <t>$126.10</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0.14</v>
+        <v>0.28</v>
       </c>
       <c r="F92" t="n">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3854,7 +3846,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>125.55 – 125.87</t>
+          <t>125.95 – 126.65</t>
         </is>
       </c>
     </row>
@@ -3874,23 +3866,23 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>102.77</t>
+          <t>100.78</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0.41</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
-        <v>0.4</v>
+        <v>1.94</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>102.72 – 102.99</t>
+          <t>100.43 – 100.95</t>
         </is>
       </c>
     </row>
@@ -3910,14 +3902,14 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>120.07</t>
+          <t>120.18</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>0.12</v>
+        <v>0.01</v>
       </c>
       <c r="F94" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -3946,14 +3938,14 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>20.99</t>
+          <t>20.49</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0.03</v>
+        <v>0.48</v>
       </c>
       <c r="F95" t="n">
-        <v>0.12</v>
+        <v>2.27</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -4062,14 +4054,14 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>$158.94</t>
+          <t>$161.82</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.66</v>
+        <v>2.88</v>
       </c>
       <c r="F98" t="n">
-        <v>0.42</v>
+        <v>1.81</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -4178,23 +4170,23 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>87.52</t>
+          <t>86.79</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.23</v>
+        <v>0.62</v>
       </c>
       <c r="F101" t="n">
-        <v>0.26</v>
+        <v>0.71</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>86.97 – 92.60</t>
+          <t>86.79 – 92.60</t>
         </is>
       </c>
     </row>
@@ -4214,14 +4206,14 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>$103.48</t>
+          <t>$103.52</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0.31</v>
+        <v>0.34</v>
       </c>
       <c r="F102" t="n">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4250,18 +4242,18 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>183.44</t>
+          <t>179.80</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.62</v>
+        <v>3.64</v>
       </c>
       <c r="F103" t="n">
-        <v>0.34</v>
+        <v>1.98</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -4326,23 +4318,23 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>374.60</t>
+          <t>367.25</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0.3</v>
+        <v>8.85</v>
       </c>
       <c r="F105" t="n">
-        <v>0.08</v>
+        <v>2.35</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>297.30 – 387.50</t>
+          <t>298.60 – 387.50</t>
         </is>
       </c>
     </row>
@@ -4362,18 +4354,18 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>225.76</t>
+          <t>217.89</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0.11</v>
+        <v>8.01</v>
       </c>
       <c r="F106" t="n">
-        <v>0.05</v>
+        <v>3.55</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -4438,18 +4430,18 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>17.47</t>
+          <t>17.24</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0.16</v>
+        <v>0.31</v>
       </c>
       <c r="F108" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.77</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -4474,14 +4466,14 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>26.67</t>
+          <t>25.85</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>0.01</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F109" t="n">
-        <v>0.04</v>
+        <v>3.04</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -4510,23 +4502,23 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>$63.68</t>
+          <t>$63.22</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.18</v>
+        <v>0.44</v>
       </c>
       <c r="F110" t="n">
-        <v>0.28</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>63.60 – 63.68</t>
+          <t>63.09 – 63.28</t>
         </is>
       </c>
     </row>
@@ -4546,14 +4538,14 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>10.65</t>
+          <t>10.88</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="F111" t="n">
-        <v>0.04</v>
+        <v>1.59</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4582,18 +4574,18 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>37.30</t>
+          <t>36.44</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0.13</v>
+        <v>0.9</v>
       </c>
       <c r="F112" t="n">
-        <v>0.34</v>
+        <v>2.42</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -4618,23 +4610,23 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>$89.44</t>
+          <t>$87.83</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>0.37</v>
+        <v>1.56</v>
       </c>
       <c r="F113" t="n">
-        <v>0.42</v>
+        <v>1.74</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>89.32 – 89.58</t>
+          <t>87.38 – 87.93</t>
         </is>
       </c>
     </row>
@@ -4654,18 +4646,18 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>35.07</t>
+          <t>34.27</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0.08</v>
+        <v>0.78</v>
       </c>
       <c r="F114" t="n">
-        <v>0.24</v>
+        <v>2.22</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -4690,14 +4682,14 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>18.32</t>
+          <t>17.77</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>0.01</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F115" t="n">
-        <v>0.03</v>
+        <v>3.05</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -4846,14 +4838,14 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>154.24</t>
+          <t>150.10</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>0.14</v>
+        <v>4.36</v>
       </c>
       <c r="F119" t="n">
-        <v>0.09</v>
+        <v>2.82</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -4922,18 +4914,18 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>58.04</t>
+          <t>56.97</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0.26</v>
+        <v>1.03</v>
       </c>
       <c r="F121" t="n">
-        <v>0.45</v>
+        <v>1.78</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -4998,18 +4990,18 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>437.95</t>
+          <t>422.46</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>0.63</v>
+        <v>15.23</v>
       </c>
       <c r="F123" t="n">
-        <v>0.14</v>
+        <v>3.48</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -5034,18 +5026,18 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>576.29</t>
+          <t>565.58</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>2.79</v>
+        <v>11.73</v>
       </c>
       <c r="F124" t="n">
-        <v>0.49</v>
+        <v>2.03</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -5070,14 +5062,14 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>524.21</t>
+          <t>515.51</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>2.33</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="F125" t="n">
-        <v>0.44</v>
+        <v>1.83</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -5146,14 +5138,14 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>267.85</t>
+          <t>253.57</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>1.27</v>
+        <v>14.67</v>
       </c>
       <c r="F127" t="n">
-        <v>0.47</v>
+        <v>5.47</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -5262,14 +5254,14 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>132.20</t>
+          <t>134.74</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>0.74</v>
+        <v>2.16</v>
       </c>
       <c r="F130" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.63</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -5378,18 +5370,18 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>16.04</t>
+          <t>15.73</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0.06</v>
+        <v>0.3</v>
       </c>
       <c r="F133" t="n">
-        <v>0.4</v>
+        <v>1.88</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -5534,18 +5526,18 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>10.90</t>
+          <t>10.71</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0.01</v>
+        <v>0.18</v>
       </c>
       <c r="F137" t="n">
-        <v>0.13</v>
+        <v>1.7</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -5690,18 +5682,18 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>26.36</t>
+          <t>25.72</t>
         </is>
       </c>
       <c r="E141" t="n">
-        <v>0.1</v>
+        <v>0.61</v>
       </c>
       <c r="F141" t="n">
-        <v>0.39</v>
+        <v>2.32</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -5766,14 +5758,14 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>18.68</t>
+          <t>18.14</t>
         </is>
       </c>
       <c r="E143" t="n">
-        <v>0.01</v>
+        <v>0.58</v>
       </c>
       <c r="F143" t="n">
-        <v>0.05</v>
+        <v>3.1</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -5882,18 +5874,18 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>43.04</t>
+          <t>42.08</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="F146" t="n">
-        <v>0.2</v>
+        <v>2.31</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -5958,18 +5950,18 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>426.17</t>
+          <t>419.27</t>
         </is>
       </c>
       <c r="E148" t="n">
-        <v>0.71</v>
+        <v>6.52</v>
       </c>
       <c r="F148" t="n">
-        <v>0.17</v>
+        <v>1.53</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -6074,18 +6066,18 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>6.14</t>
+          <t>6.17</t>
         </is>
       </c>
       <c r="E151" t="n">
         <v>0.01</v>
       </c>
       <c r="F151" t="n">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -6230,18 +6222,18 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>283.65</t>
+          <t>277.28</t>
         </is>
       </c>
       <c r="E155" t="n">
-        <v>0.38</v>
+        <v>6.74</v>
       </c>
       <c r="F155" t="n">
-        <v>0.13</v>
+        <v>2.37</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
@@ -6266,14 +6258,14 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>63.54</t>
+          <t>63.70</t>
         </is>
       </c>
       <c r="E156" t="n">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="F156" t="n">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
@@ -6302,14 +6294,18 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>$31.27</t>
-        </is>
-      </c>
-      <c r="E157" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="F157" t="n">
-        <v>0.79</v>
+          <t>Check manually</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Check manually</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Check manually</t>
+        </is>
       </c>
       <c r="G157" t="inlineStr">
         <is>
@@ -6338,23 +6334,23 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>$20.74</t>
+          <t>$20.46</t>
         </is>
       </c>
       <c r="E158" t="n">
-        <v>0.04</v>
+        <v>0.33</v>
       </c>
       <c r="F158" t="n">
-        <v>0.19</v>
+        <v>1.59</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>20.59 – 20.71</t>
+          <t>20.46 – 20.46</t>
         </is>
       </c>
     </row>
@@ -6374,18 +6370,18 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>$7.14</t>
+          <t>$7.08</t>
         </is>
       </c>
       <c r="E159" t="n">
         <v>0.04</v>
       </c>
       <c r="F159" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -6410,18 +6406,18 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>265.55</t>
+          <t>260.00</t>
         </is>
       </c>
       <c r="E160" t="n">
-        <v>0.87</v>
+        <v>5.85</v>
       </c>
       <c r="F160" t="n">
-        <v>0.33</v>
+        <v>2.2</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -6446,18 +6442,18 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>178.47</t>
+          <t>175.35</t>
         </is>
       </c>
       <c r="E161" t="n">
-        <v>0.22</v>
+        <v>3.17</v>
       </c>
       <c r="F161" t="n">
-        <v>0.12</v>
+        <v>1.78</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -6482,18 +6478,18 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>426.17</t>
+          <t>419.27</t>
         </is>
       </c>
       <c r="E162" t="n">
-        <v>0.71</v>
+        <v>6.52</v>
       </c>
       <c r="F162" t="n">
-        <v>0.17</v>
+        <v>1.53</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
@@ -6518,23 +6514,23 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>$85.88</t>
+          <t>$84.57</t>
         </is>
       </c>
       <c r="E163" t="n">
-        <v>0.14</v>
+        <v>1.63</v>
       </c>
       <c r="F163" t="n">
-        <v>0.16</v>
+        <v>1.89</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>85.63 – 85.90</t>
+          <t>84.57 – 84.57</t>
         </is>
       </c>
     </row>
@@ -6554,23 +6550,23 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>$88.58</t>
+          <t>$86.91</t>
         </is>
       </c>
       <c r="E164" t="n">
-        <v>0.43</v>
+        <v>1.62</v>
       </c>
       <c r="F164" t="n">
-        <v>0.49</v>
+        <v>1.83</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>88.44 – 88.71</t>
+          <t>86.40 – 87.59</t>
         </is>
       </c>
     </row>
@@ -6590,18 +6586,18 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>20.21</t>
+          <t>19.75</t>
         </is>
       </c>
       <c r="E165" t="n">
-        <v>0.05</v>
+        <v>0.47</v>
       </c>
       <c r="F165" t="n">
-        <v>0.24</v>
+        <v>2.32</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
@@ -6626,18 +6622,18 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>34.24</t>
+          <t>33.57</t>
         </is>
       </c>
       <c r="E166" t="n">
-        <v>0.1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F166" t="n">
-        <v>0.3</v>
+        <v>2.01</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -6662,18 +6658,18 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>11.72</t>
+          <t>11.37</t>
         </is>
       </c>
       <c r="E167" t="n">
-        <v>0.01</v>
+        <v>0.37</v>
       </c>
       <c r="F167" t="n">
-        <v>0.11</v>
+        <v>3.15</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -6698,23 +6694,23 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>$66.93</t>
+          <t>$65.74</t>
         </is>
       </c>
       <c r="E168" t="n">
-        <v>0.58</v>
+        <v>1.2</v>
       </c>
       <c r="F168" t="n">
-        <v>0.87</v>
+        <v>1.79</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>66.79 – 67.03</t>
+          <t>65.38 – 66.01</t>
         </is>
       </c>
     </row>

</xml_diff>